<commit_message>
add hours saved counter and improve responsive
</commit_message>
<xml_diff>
--- a/app/automations/a2/downloads/fundraising_template.xlsx
+++ b/app/automations/a2/downloads/fundraising_template.xlsx
@@ -2700,4610 +2700,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Thème Office">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:srgbClr val="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:srgbClr val="ffffff"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546a"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ed7d31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="ffc000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472c4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70ad47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563c1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954f72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme>
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-</a:theme>
-</file>
-
-<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AU43"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 0</t>
-        </is>
-      </c>
-      <c r="B1" s="441" t="inlineStr">
-        <is>
-          <t>Weekending</t>
-        </is>
-      </c>
-      <c r="C1" s="443" t="n">
-        <v>45613</v>
-      </c>
-      <c r="D1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 3</t>
-        </is>
-      </c>
-      <c r="E1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 4</t>
-        </is>
-      </c>
-      <c r="F1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 5</t>
-        </is>
-      </c>
-      <c r="G1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 6</t>
-        </is>
-      </c>
-      <c r="H1" s="441" t="n">
-        <v>0.7057943831494483</v>
-      </c>
-      <c r="I1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 8</t>
-        </is>
-      </c>
-      <c r="J1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 9</t>
-        </is>
-      </c>
-      <c r="K1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 10</t>
-        </is>
-      </c>
-      <c r="L1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 11</t>
-        </is>
-      </c>
-      <c r="M1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 12</t>
-        </is>
-      </c>
-      <c r="N1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 13</t>
-        </is>
-      </c>
-      <c r="O1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 14</t>
-        </is>
-      </c>
-      <c r="P1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 15</t>
-        </is>
-      </c>
-      <c r="Q1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 16</t>
-        </is>
-      </c>
-      <c r="R1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 17</t>
-        </is>
-      </c>
-      <c r="S1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 18</t>
-        </is>
-      </c>
-      <c r="T1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 19</t>
-        </is>
-      </c>
-      <c r="U1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 20</t>
-        </is>
-      </c>
-      <c r="V1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 21</t>
-        </is>
-      </c>
-      <c r="W1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 22</t>
-        </is>
-      </c>
-      <c r="X1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 23</t>
-        </is>
-      </c>
-      <c r="Y1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 24</t>
-        </is>
-      </c>
-      <c r="Z1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 25</t>
-        </is>
-      </c>
-      <c r="AA1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 26</t>
-        </is>
-      </c>
-      <c r="AB1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 27</t>
-        </is>
-      </c>
-      <c r="AC1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 28</t>
-        </is>
-      </c>
-      <c r="AD1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 29</t>
-        </is>
-      </c>
-      <c r="AE1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 30</t>
-        </is>
-      </c>
-      <c r="AF1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 31</t>
-        </is>
-      </c>
-      <c r="AG1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 32</t>
-        </is>
-      </c>
-      <c r="AH1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 33</t>
-        </is>
-      </c>
-      <c r="AI1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 34</t>
-        </is>
-      </c>
-      <c r="AJ1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 35</t>
-        </is>
-      </c>
-      <c r="AK1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 36</t>
-        </is>
-      </c>
-      <c r="AL1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 37</t>
-        </is>
-      </c>
-      <c r="AM1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 38</t>
-        </is>
-      </c>
-      <c r="AN1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 39</t>
-        </is>
-      </c>
-      <c r="AO1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 40</t>
-        </is>
-      </c>
-      <c r="AP1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 41</t>
-        </is>
-      </c>
-      <c r="AQ1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 42</t>
-        </is>
-      </c>
-      <c r="AR1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 43</t>
-        </is>
-      </c>
-      <c r="AS1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 44</t>
-        </is>
-      </c>
-      <c r="AT1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 45</t>
-        </is>
-      </c>
-      <c r="AU1" s="441" t="inlineStr">
-        <is>
-          <t>Unnamed: 46</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>TeamNumber</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Result MC</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr"/>
-      <c r="V2" t="inlineStr"/>
-      <c r="W2" t="inlineStr"/>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="inlineStr"/>
-      <c r="AD2" t="inlineStr"/>
-      <c r="AE2" t="inlineStr"/>
-      <c r="AF2" t="inlineStr"/>
-      <c r="AG2" t="inlineStr"/>
-      <c r="AH2" t="inlineStr"/>
-      <c r="AI2" t="inlineStr"/>
-      <c r="AJ2" t="inlineStr"/>
-      <c r="AK2" t="inlineStr"/>
-      <c r="AL2" t="inlineStr"/>
-      <c r="AM2" t="inlineStr"/>
-      <c r="AN2" t="inlineStr"/>
-      <c r="AO2" t="inlineStr"/>
-      <c r="AP2" t="inlineStr"/>
-      <c r="AQ2" t="inlineStr"/>
-      <c r="AR2" t="inlineStr"/>
-      <c r="AS2" t="inlineStr"/>
-      <c r="AT2" t="inlineStr"/>
-      <c r="AU2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>MC Name</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>DLG Corporation</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Numbers</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Fees</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Amount</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Challenge(s)</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>Value Challenge(s)</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="inlineStr"/>
-      <c r="AD3" t="inlineStr"/>
-      <c r="AE3" t="inlineStr"/>
-      <c r="AF3" t="inlineStr"/>
-      <c r="AG3" t="inlineStr"/>
-      <c r="AH3" t="inlineStr"/>
-      <c r="AI3" t="inlineStr"/>
-      <c r="AJ3" t="inlineStr"/>
-      <c r="AK3" t="inlineStr"/>
-      <c r="AL3" t="inlineStr"/>
-      <c r="AM3" t="inlineStr"/>
-      <c r="AN3" t="inlineStr"/>
-      <c r="AO3" t="inlineStr"/>
-      <c r="AP3" t="inlineStr"/>
-      <c r="AQ3" t="inlineStr"/>
-      <c r="AR3" t="inlineStr"/>
-      <c r="AS3" t="inlineStr"/>
-      <c r="AT3" t="inlineStr"/>
-      <c r="AU3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr"/>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Campaign Type</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Fundraising</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Sales - TOTAL</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
-      <c r="V4" t="inlineStr"/>
-      <c r="W4" t="inlineStr"/>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="inlineStr"/>
-      <c r="AB4" t="inlineStr"/>
-      <c r="AC4" t="inlineStr"/>
-      <c r="AD4" t="inlineStr"/>
-      <c r="AE4" t="inlineStr"/>
-      <c r="AF4" t="inlineStr"/>
-      <c r="AG4" t="inlineStr"/>
-      <c r="AH4" t="inlineStr"/>
-      <c r="AI4" t="inlineStr"/>
-      <c r="AJ4" t="inlineStr"/>
-      <c r="AK4" t="inlineStr"/>
-      <c r="AL4" t="inlineStr"/>
-      <c r="AM4" t="inlineStr"/>
-      <c r="AN4" t="inlineStr"/>
-      <c r="AO4" t="inlineStr"/>
-      <c r="AP4" t="inlineStr"/>
-      <c r="AQ4" t="inlineStr"/>
-      <c r="AR4" t="inlineStr"/>
-      <c r="AS4" t="inlineStr"/>
-      <c r="AT4" t="inlineStr"/>
-      <c r="AU4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr"/>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Campaign Name</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Croix-Rouge</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Sales - Fail</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr"/>
-      <c r="V5" t="inlineStr"/>
-      <c r="W5" t="inlineStr"/>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="inlineStr"/>
-      <c r="AB5" t="inlineStr"/>
-      <c r="AC5" t="inlineStr"/>
-      <c r="AD5" t="inlineStr"/>
-      <c r="AE5" t="inlineStr"/>
-      <c r="AF5" t="inlineStr"/>
-      <c r="AG5" t="inlineStr"/>
-      <c r="AH5" t="inlineStr"/>
-      <c r="AI5" t="inlineStr"/>
-      <c r="AJ5" t="inlineStr"/>
-      <c r="AK5" t="inlineStr"/>
-      <c r="AL5" t="inlineStr"/>
-      <c r="AM5" t="inlineStr"/>
-      <c r="AN5" t="inlineStr"/>
-      <c r="AO5" t="inlineStr"/>
-      <c r="AP5" t="inlineStr"/>
-      <c r="AQ5" t="inlineStr"/>
-      <c r="AR5" t="inlineStr"/>
-      <c r="AS5" t="inlineStr"/>
-      <c r="AT5" t="inlineStr"/>
-      <c r="AU5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Sales - Submission</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
-      <c r="V6" t="inlineStr"/>
-      <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="inlineStr"/>
-      <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="inlineStr"/>
-      <c r="AD6" t="inlineStr"/>
-      <c r="AE6" t="inlineStr"/>
-      <c r="AF6" t="inlineStr"/>
-      <c r="AG6" t="inlineStr"/>
-      <c r="AH6" t="inlineStr"/>
-      <c r="AI6" t="inlineStr"/>
-      <c r="AJ6" t="inlineStr"/>
-      <c r="AK6" t="inlineStr"/>
-      <c r="AL6" t="inlineStr"/>
-      <c r="AM6" t="inlineStr"/>
-      <c r="AN6" t="inlineStr"/>
-      <c r="AO6" t="inlineStr"/>
-      <c r="AP6" t="inlineStr"/>
-      <c r="AQ6" t="inlineStr"/>
-      <c r="AR6" t="inlineStr"/>
-      <c r="AS6" t="inlineStr"/>
-      <c r="AT6" t="inlineStr"/>
-      <c r="AU6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
-      <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="inlineStr"/>
-      <c r="AB7" t="inlineStr"/>
-      <c r="AC7" t="inlineStr"/>
-      <c r="AD7" t="inlineStr"/>
-      <c r="AE7" t="inlineStr"/>
-      <c r="AF7" t="inlineStr"/>
-      <c r="AG7" t="inlineStr"/>
-      <c r="AH7" t="inlineStr"/>
-      <c r="AI7" t="inlineStr"/>
-      <c r="AJ7" t="inlineStr"/>
-      <c r="AK7" t="inlineStr"/>
-      <c r="AL7" t="inlineStr"/>
-      <c r="AM7" t="inlineStr"/>
-      <c r="AN7" t="inlineStr"/>
-      <c r="AO7" t="inlineStr"/>
-      <c r="AP7" t="inlineStr"/>
-      <c r="AQ7" t="inlineStr"/>
-      <c r="AR7" t="inlineStr"/>
-      <c r="AS7" t="inlineStr"/>
-      <c r="AT7" t="inlineStr"/>
-      <c r="AU7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Quality Return Balance</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="n">
-        <v>-0.2942056168505517</v>
-      </c>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
-      <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr"/>
-      <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="inlineStr"/>
-      <c r="AD8" t="inlineStr"/>
-      <c r="AE8" t="inlineStr"/>
-      <c r="AF8" t="inlineStr"/>
-      <c r="AG8" t="inlineStr"/>
-      <c r="AH8" t="inlineStr"/>
-      <c r="AI8" t="inlineStr"/>
-      <c r="AJ8" t="inlineStr"/>
-      <c r="AK8" t="inlineStr"/>
-      <c r="AL8" t="inlineStr"/>
-      <c r="AM8" t="inlineStr"/>
-      <c r="AN8" t="inlineStr"/>
-      <c r="AO8" t="inlineStr"/>
-      <c r="AP8" t="inlineStr"/>
-      <c r="AQ8" t="inlineStr"/>
-      <c r="AR8" t="inlineStr"/>
-      <c r="AS8" t="inlineStr"/>
-      <c r="AT8" t="inlineStr"/>
-      <c r="AU8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
-      <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr"/>
-      <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="inlineStr"/>
-      <c r="AD9" t="inlineStr"/>
-      <c r="AE9" t="inlineStr"/>
-      <c r="AF9" t="inlineStr"/>
-      <c r="AG9" t="inlineStr"/>
-      <c r="AH9" t="inlineStr"/>
-      <c r="AI9" t="inlineStr"/>
-      <c r="AJ9" t="inlineStr"/>
-      <c r="AK9" t="inlineStr"/>
-      <c r="AL9" t="inlineStr"/>
-      <c r="AM9" t="inlineStr"/>
-      <c r="AN9" t="inlineStr"/>
-      <c r="AO9" t="inlineStr"/>
-      <c r="AP9" t="inlineStr"/>
-      <c r="AQ9" t="inlineStr"/>
-      <c r="AR9" t="inlineStr"/>
-      <c r="AS9" t="inlineStr"/>
-      <c r="AT9" t="inlineStr"/>
-      <c r="AU9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Quality Return MC</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
-      <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="inlineStr"/>
-      <c r="AC10" t="inlineStr"/>
-      <c r="AD10" t="inlineStr"/>
-      <c r="AE10" t="inlineStr"/>
-      <c r="AF10" t="inlineStr"/>
-      <c r="AG10" t="inlineStr"/>
-      <c r="AH10" t="inlineStr"/>
-      <c r="AI10" t="inlineStr"/>
-      <c r="AJ10" t="inlineStr"/>
-      <c r="AK10" t="inlineStr"/>
-      <c r="AL10" t="inlineStr"/>
-      <c r="AM10" t="inlineStr"/>
-      <c r="AN10" t="inlineStr"/>
-      <c r="AO10" t="inlineStr"/>
-      <c r="AP10" t="inlineStr"/>
-      <c r="AQ10" t="inlineStr"/>
-      <c r="AR10" t="inlineStr"/>
-      <c r="AS10" t="inlineStr"/>
-      <c r="AT10" t="inlineStr"/>
-      <c r="AU10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Total movement quality balance</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="n">
-        <v>-8073</v>
-      </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
-      <c r="V11" t="inlineStr"/>
-      <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="inlineStr"/>
-      <c r="AA11" t="inlineStr"/>
-      <c r="AB11" t="inlineStr"/>
-      <c r="AC11" t="inlineStr"/>
-      <c r="AD11" t="inlineStr"/>
-      <c r="AE11" t="inlineStr"/>
-      <c r="AF11" t="inlineStr"/>
-      <c r="AG11" t="inlineStr"/>
-      <c r="AH11" t="inlineStr"/>
-      <c r="AI11" t="inlineStr"/>
-      <c r="AJ11" t="inlineStr"/>
-      <c r="AK11" t="inlineStr"/>
-      <c r="AL11" t="inlineStr"/>
-      <c r="AM11" t="inlineStr"/>
-      <c r="AN11" t="inlineStr"/>
-      <c r="AO11" t="inlineStr"/>
-      <c r="AP11" t="inlineStr"/>
-      <c r="AQ11" t="inlineStr"/>
-      <c r="AR11" t="inlineStr"/>
-      <c r="AS11" t="inlineStr"/>
-      <c r="AT11" t="inlineStr"/>
-      <c r="AU11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Total paid to MC</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
-      <c r="V12" t="inlineStr"/>
-      <c r="W12" t="inlineStr"/>
-      <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
-      <c r="Z12" t="inlineStr"/>
-      <c r="AA12" t="inlineStr"/>
-      <c r="AB12" t="inlineStr"/>
-      <c r="AC12" t="inlineStr"/>
-      <c r="AD12" t="inlineStr"/>
-      <c r="AE12" t="inlineStr"/>
-      <c r="AF12" t="inlineStr"/>
-      <c r="AG12" t="inlineStr"/>
-      <c r="AH12" t="inlineStr"/>
-      <c r="AI12" t="inlineStr"/>
-      <c r="AJ12" t="inlineStr"/>
-      <c r="AK12" t="inlineStr"/>
-      <c r="AL12" t="inlineStr"/>
-      <c r="AM12" t="inlineStr"/>
-      <c r="AN12" t="inlineStr"/>
-      <c r="AO12" t="inlineStr"/>
-      <c r="AP12" t="inlineStr"/>
-      <c r="AQ12" t="inlineStr"/>
-      <c r="AR12" t="inlineStr"/>
-      <c r="AS12" t="inlineStr"/>
-      <c r="AT12" t="inlineStr"/>
-      <c r="AU12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
-      <c r="V13" t="inlineStr"/>
-      <c r="W13" t="inlineStr"/>
-      <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="inlineStr"/>
-      <c r="AD13" t="inlineStr"/>
-      <c r="AE13" t="inlineStr"/>
-      <c r="AF13" t="inlineStr"/>
-      <c r="AG13" t="inlineStr"/>
-      <c r="AH13" t="inlineStr"/>
-      <c r="AI13" t="inlineStr"/>
-      <c r="AJ13" t="inlineStr"/>
-      <c r="AK13" t="inlineStr"/>
-      <c r="AL13" t="inlineStr"/>
-      <c r="AM13" t="inlineStr"/>
-      <c r="AN13" t="inlineStr"/>
-      <c r="AO13" t="inlineStr"/>
-      <c r="AP13" t="inlineStr"/>
-      <c r="AQ13" t="inlineStr"/>
-      <c r="AR13" t="inlineStr"/>
-      <c r="AS13" t="inlineStr"/>
-      <c r="AT13" t="inlineStr"/>
-      <c r="AU13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
-      <c r="K14" t="inlineStr"/>
-      <c r="L14" t="inlineStr"/>
-      <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr"/>
-      <c r="O14" t="inlineStr"/>
-      <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr"/>
-      <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
-      <c r="T14" t="inlineStr"/>
-      <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
-      <c r="W14" t="inlineStr"/>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="inlineStr"/>
-      <c r="AA14" t="inlineStr"/>
-      <c r="AB14" t="inlineStr"/>
-      <c r="AC14" t="inlineStr"/>
-      <c r="AD14" t="inlineStr"/>
-      <c r="AE14" t="inlineStr"/>
-      <c r="AF14" t="inlineStr"/>
-      <c r="AG14" t="inlineStr"/>
-      <c r="AH14" t="inlineStr"/>
-      <c r="AI14" t="inlineStr"/>
-      <c r="AJ14" t="inlineStr"/>
-      <c r="AK14" t="inlineStr"/>
-      <c r="AL14" t="inlineStr"/>
-      <c r="AM14" t="inlineStr"/>
-      <c r="AN14" t="inlineStr"/>
-      <c r="AO14" t="inlineStr"/>
-      <c r="AP14" t="inlineStr"/>
-      <c r="AQ14" t="inlineStr"/>
-      <c r="AR14" t="inlineStr"/>
-      <c r="AS14" t="inlineStr"/>
-      <c r="AT14" t="inlineStr"/>
-      <c r="AU14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr"/>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Total Sales</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>Total Failed Forms</t>
-        </is>
-      </c>
-      <c r="P15" t="inlineStr"/>
-      <c r="Q15" t="inlineStr"/>
-      <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
-      <c r="T15" t="inlineStr">
-        <is>
-          <t>Total Submissions</t>
-        </is>
-      </c>
-      <c r="U15" t="inlineStr"/>
-      <c r="V15" t="inlineStr"/>
-      <c r="W15" t="inlineStr"/>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr">
-        <is>
-          <t>BA Fees</t>
-        </is>
-      </c>
-      <c r="Z15" t="inlineStr"/>
-      <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="inlineStr"/>
-      <c r="AC15" t="inlineStr"/>
-      <c r="AD15" t="inlineStr"/>
-      <c r="AE15" t="inlineStr"/>
-      <c r="AF15" t="inlineStr"/>
-      <c r="AG15" t="inlineStr">
-        <is>
-          <t>Rejects</t>
-        </is>
-      </c>
-      <c r="AH15" t="inlineStr"/>
-      <c r="AI15" t="inlineStr"/>
-      <c r="AJ15" t="inlineStr"/>
-      <c r="AK15" t="inlineStr">
-        <is>
-          <t>Bonus</t>
-        </is>
-      </c>
-      <c r="AL15" t="inlineStr"/>
-      <c r="AM15" t="inlineStr"/>
-      <c r="AN15" t="inlineStr"/>
-      <c r="AO15" t="inlineStr"/>
-      <c r="AP15" t="inlineStr">
-        <is>
-          <t>Deductions</t>
-        </is>
-      </c>
-      <c r="AQ15" t="inlineStr"/>
-      <c r="AR15" t="inlineStr"/>
-      <c r="AS15" t="inlineStr"/>
-      <c r="AT15" t="inlineStr"/>
-      <c r="AU15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr"/>
-      <c r="J16" t="n">
-        <v>0</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>0</v>
-      </c>
-      <c r="R16" t="n">
-        <v>0</v>
-      </c>
-      <c r="S16" t="n">
-        <v>0</v>
-      </c>
-      <c r="T16" t="n">
-        <v>0</v>
-      </c>
-      <c r="U16" t="n">
-        <v>0</v>
-      </c>
-      <c r="V16" t="n">
-        <v>0</v>
-      </c>
-      <c r="W16" t="n">
-        <v>0</v>
-      </c>
-      <c r="X16" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="inlineStr"/>
-      <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD16" t="inlineStr"/>
-      <c r="AE16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG16" t="n">
-        <v>69</v>
-      </c>
-      <c r="AH16" t="n">
-        <v>2723</v>
-      </c>
-      <c r="AI16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ16" t="n">
-        <v>-2723</v>
-      </c>
-      <c r="AK16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AL16" t="inlineStr"/>
-      <c r="AM16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN16" t="inlineStr"/>
-      <c r="AO16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AQ16" t="inlineStr"/>
-      <c r="AR16" t="inlineStr"/>
-      <c r="AS16" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT16" t="inlineStr"/>
-      <c r="AU16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>MAX</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>TeamNumber</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>BANumber</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>BAName</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>BAStartDate</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>BAStatus</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Statut Commission</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Total Sales since BA Start Date</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Total Sales since Campaign Start Date</t>
-        </is>
-      </c>
-      <c r="J17" t="n">
-        <v>10</v>
-      </c>
-      <c r="K17" t="n">
-        <v>15</v>
-      </c>
-      <c r="L17" t="n">
-        <v>20</v>
-      </c>
-      <c r="M17" t="n">
-        <v>25</v>
-      </c>
-      <c r="N17" t="inlineStr">
-        <is>
-          <t>Total Sales</t>
-        </is>
-      </c>
-      <c r="O17" t="n">
-        <v>10</v>
-      </c>
-      <c r="P17" t="n">
-        <v>15</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>20</v>
-      </c>
-      <c r="R17" t="n">
-        <v>25</v>
-      </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>Total Fails</t>
-        </is>
-      </c>
-      <c r="T17" t="n">
-        <v>10</v>
-      </c>
-      <c r="U17" t="n">
-        <v>15</v>
-      </c>
-      <c r="V17" t="n">
-        <v>20</v>
-      </c>
-      <c r="W17" t="n">
-        <v>25</v>
-      </c>
-      <c r="X17" t="inlineStr">
-        <is>
-          <t>Total Submissions</t>
-        </is>
-      </c>
-      <c r="Y17" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>15</v>
-      </c>
-      <c r="AA17" t="n">
-        <v>20</v>
-      </c>
-      <c r="AB17" t="n">
-        <v>25</v>
-      </c>
-      <c r="AC17" t="inlineStr">
-        <is>
-          <t>Total BA Fees</t>
-        </is>
-      </c>
-      <c r="AD17" t="inlineStr">
-        <is>
-          <t>Prepayment Percentage</t>
-        </is>
-      </c>
-      <c r="AE17" t="inlineStr">
-        <is>
-          <t>Prepayment Amount</t>
-        </is>
-      </c>
-      <c r="AF17" t="inlineStr">
-        <is>
-          <t>Amount add to bond</t>
-        </is>
-      </c>
-      <c r="AG17" t="inlineStr">
-        <is>
-          <t>Sales rejected</t>
-        </is>
-      </c>
-      <c r="AH17" t="inlineStr">
-        <is>
-          <t>Reject value sales</t>
-        </is>
-      </c>
-      <c r="AI17" t="inlineStr">
-        <is>
-          <t>Quality balance return</t>
-        </is>
-      </c>
-      <c r="AJ17" t="inlineStr">
-        <is>
-          <t>Total quality balance movement</t>
-        </is>
-      </c>
-      <c r="AK17" t="inlineStr">
-        <is>
-          <t>Amount</t>
-        </is>
-      </c>
-      <c r="AL17" t="inlineStr">
-        <is>
-          <t>Comment 1
-REQUIRED</t>
-        </is>
-      </c>
-      <c r="AM17" t="inlineStr">
-        <is>
-          <t>Amount For Social Security Calculation</t>
-        </is>
-      </c>
-      <c r="AN17" t="inlineStr">
-        <is>
-          <t>Social Security percentage</t>
-        </is>
-      </c>
-      <c r="AO17" t="inlineStr">
-        <is>
-          <t>Amount Social Security Deductions</t>
-        </is>
-      </c>
-      <c r="AP17" t="inlineStr">
-        <is>
-          <t>Amount
-(to be set in negative)</t>
-        </is>
-      </c>
-      <c r="AQ17" t="inlineStr">
-        <is>
-          <t>Comment 1
-REQUIRED</t>
-        </is>
-      </c>
-      <c r="AR17" t="inlineStr">
-        <is>
-          <t>Comment 2
-to be completed if Comment 1 = 'Other'.</t>
-        </is>
-      </c>
-      <c r="AS17" t="inlineStr">
-        <is>
-          <t>Total Payment</t>
-        </is>
-      </c>
-      <c r="AT17" t="inlineStr">
-        <is>
-          <t>Formule Commentaire</t>
-        </is>
-      </c>
-      <c r="AU17" t="inlineStr">
-        <is>
-          <t>Pour Fees</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>18</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>29827</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
-      <c r="I18" t="inlineStr"/>
-      <c r="J18" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" t="n">
-        <v>0</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0</v>
-      </c>
-      <c r="N18" t="n">
-        <v>0</v>
-      </c>
-      <c r="O18" t="n">
-        <v>0</v>
-      </c>
-      <c r="P18" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>0</v>
-      </c>
-      <c r="R18" t="n">
-        <v>0</v>
-      </c>
-      <c r="S18" t="n">
-        <v>0</v>
-      </c>
-      <c r="T18" t="n">
-        <v>0</v>
-      </c>
-      <c r="U18" t="n">
-        <v>0</v>
-      </c>
-      <c r="V18" t="n">
-        <v>0</v>
-      </c>
-      <c r="W18" t="n">
-        <v>0</v>
-      </c>
-      <c r="X18" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y18" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD18" t="inlineStr"/>
-      <c r="AE18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG18" t="n">
-        <v>4</v>
-      </c>
-      <c r="AH18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI18" t="inlineStr"/>
-      <c r="AJ18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK18" t="inlineStr"/>
-      <c r="AL18" t="inlineStr"/>
-      <c r="AM18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN18" t="inlineStr"/>
-      <c r="AO18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP18" t="inlineStr"/>
-      <c r="AQ18" t="inlineStr"/>
-      <c r="AR18" t="inlineStr"/>
-      <c r="AS18" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT18" t="inlineStr"/>
-      <c r="AU18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>19</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>30311</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr"/>
-      <c r="J19" t="n">
-        <v>0</v>
-      </c>
-      <c r="K19" t="n">
-        <v>0</v>
-      </c>
-      <c r="L19" t="n">
-        <v>0</v>
-      </c>
-      <c r="M19" t="n">
-        <v>0</v>
-      </c>
-      <c r="N19" t="n">
-        <v>0</v>
-      </c>
-      <c r="O19" t="n">
-        <v>0</v>
-      </c>
-      <c r="P19" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q19" t="n">
-        <v>0</v>
-      </c>
-      <c r="R19" t="n">
-        <v>0</v>
-      </c>
-      <c r="S19" t="n">
-        <v>0</v>
-      </c>
-      <c r="T19" t="n">
-        <v>0</v>
-      </c>
-      <c r="U19" t="n">
-        <v>0</v>
-      </c>
-      <c r="V19" t="n">
-        <v>0</v>
-      </c>
-      <c r="W19" t="n">
-        <v>0</v>
-      </c>
-      <c r="X19" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y19" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD19" t="inlineStr"/>
-      <c r="AE19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG19" t="n">
-        <v>14</v>
-      </c>
-      <c r="AH19" t="n">
-        <v>650</v>
-      </c>
-      <c r="AI19" t="inlineStr"/>
-      <c r="AJ19" t="n">
-        <v>-650</v>
-      </c>
-      <c r="AK19" t="inlineStr"/>
-      <c r="AL19" t="inlineStr"/>
-      <c r="AM19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN19" t="inlineStr"/>
-      <c r="AO19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP19" t="inlineStr"/>
-      <c r="AQ19" t="inlineStr"/>
-      <c r="AR19" t="inlineStr"/>
-      <c r="AS19" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT19" t="inlineStr"/>
-      <c r="AU19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>20</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>30840</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr"/>
-      <c r="J20" t="n">
-        <v>0</v>
-      </c>
-      <c r="K20" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" t="n">
-        <v>0</v>
-      </c>
-      <c r="M20" t="n">
-        <v>0</v>
-      </c>
-      <c r="N20" t="n">
-        <v>0</v>
-      </c>
-      <c r="O20" t="n">
-        <v>0</v>
-      </c>
-      <c r="P20" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q20" t="n">
-        <v>0</v>
-      </c>
-      <c r="R20" t="n">
-        <v>0</v>
-      </c>
-      <c r="S20" t="n">
-        <v>0</v>
-      </c>
-      <c r="T20" t="n">
-        <v>0</v>
-      </c>
-      <c r="U20" t="n">
-        <v>0</v>
-      </c>
-      <c r="V20" t="n">
-        <v>0</v>
-      </c>
-      <c r="W20" t="n">
-        <v>0</v>
-      </c>
-      <c r="X20" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y20" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD20" t="inlineStr"/>
-      <c r="AE20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG20" t="n">
-        <v>7</v>
-      </c>
-      <c r="AH20" t="n">
-        <v>315</v>
-      </c>
-      <c r="AI20" t="inlineStr"/>
-      <c r="AJ20" t="n">
-        <v>-315</v>
-      </c>
-      <c r="AK20" t="inlineStr"/>
-      <c r="AL20" t="inlineStr"/>
-      <c r="AM20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN20" t="inlineStr"/>
-      <c r="AO20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP20" t="inlineStr"/>
-      <c r="AQ20" t="inlineStr"/>
-      <c r="AR20" t="inlineStr"/>
-      <c r="AS20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT20" t="inlineStr"/>
-      <c r="AU20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>21</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>31648</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr"/>
-      <c r="J21" t="n">
-        <v>0</v>
-      </c>
-      <c r="K21" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" t="n">
-        <v>0</v>
-      </c>
-      <c r="M21" t="n">
-        <v>0</v>
-      </c>
-      <c r="N21" t="n">
-        <v>0</v>
-      </c>
-      <c r="O21" t="n">
-        <v>0</v>
-      </c>
-      <c r="P21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>0</v>
-      </c>
-      <c r="R21" t="n">
-        <v>0</v>
-      </c>
-      <c r="S21" t="n">
-        <v>0</v>
-      </c>
-      <c r="T21" t="n">
-        <v>0</v>
-      </c>
-      <c r="U21" t="n">
-        <v>0</v>
-      </c>
-      <c r="V21" t="n">
-        <v>0</v>
-      </c>
-      <c r="W21" t="n">
-        <v>0</v>
-      </c>
-      <c r="X21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD21" t="inlineStr"/>
-      <c r="AE21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG21" t="n">
-        <v>4</v>
-      </c>
-      <c r="AH21" t="n">
-        <v>175</v>
-      </c>
-      <c r="AI21" t="inlineStr"/>
-      <c r="AJ21" t="n">
-        <v>-175</v>
-      </c>
-      <c r="AK21" t="inlineStr"/>
-      <c r="AL21" t="inlineStr"/>
-      <c r="AM21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN21" t="inlineStr"/>
-      <c r="AO21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP21" t="inlineStr"/>
-      <c r="AQ21" t="inlineStr"/>
-      <c r="AR21" t="inlineStr"/>
-      <c r="AS21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT21" t="inlineStr"/>
-      <c r="AU21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
-        <v>22</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>32068</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
-      <c r="I22" t="inlineStr"/>
-      <c r="J22" t="n">
-        <v>0</v>
-      </c>
-      <c r="K22" t="n">
-        <v>0</v>
-      </c>
-      <c r="L22" t="n">
-        <v>0</v>
-      </c>
-      <c r="M22" t="n">
-        <v>0</v>
-      </c>
-      <c r="N22" t="n">
-        <v>0</v>
-      </c>
-      <c r="O22" t="n">
-        <v>0</v>
-      </c>
-      <c r="P22" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q22" t="n">
-        <v>0</v>
-      </c>
-      <c r="R22" t="n">
-        <v>0</v>
-      </c>
-      <c r="S22" t="n">
-        <v>0</v>
-      </c>
-      <c r="T22" t="n">
-        <v>0</v>
-      </c>
-      <c r="U22" t="n">
-        <v>0</v>
-      </c>
-      <c r="V22" t="n">
-        <v>0</v>
-      </c>
-      <c r="W22" t="n">
-        <v>0</v>
-      </c>
-      <c r="X22" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y22" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD22" t="inlineStr"/>
-      <c r="AE22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG22" t="n">
-        <v>2</v>
-      </c>
-      <c r="AH22" t="n">
-        <v>73</v>
-      </c>
-      <c r="AI22" t="inlineStr"/>
-      <c r="AJ22" t="n">
-        <v>-73</v>
-      </c>
-      <c r="AK22" t="inlineStr"/>
-      <c r="AL22" t="inlineStr"/>
-      <c r="AM22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN22" t="inlineStr"/>
-      <c r="AO22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP22" t="inlineStr"/>
-      <c r="AQ22" t="inlineStr"/>
-      <c r="AR22" t="inlineStr"/>
-      <c r="AS22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT22" t="inlineStr"/>
-      <c r="AU22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
-        <v>23</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>32069</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-      <c r="I23" t="inlineStr"/>
-      <c r="J23" t="n">
-        <v>0</v>
-      </c>
-      <c r="K23" t="n">
-        <v>0</v>
-      </c>
-      <c r="L23" t="n">
-        <v>0</v>
-      </c>
-      <c r="M23" t="n">
-        <v>0</v>
-      </c>
-      <c r="N23" t="n">
-        <v>0</v>
-      </c>
-      <c r="O23" t="n">
-        <v>0</v>
-      </c>
-      <c r="P23" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q23" t="n">
-        <v>0</v>
-      </c>
-      <c r="R23" t="n">
-        <v>0</v>
-      </c>
-      <c r="S23" t="n">
-        <v>0</v>
-      </c>
-      <c r="T23" t="n">
-        <v>0</v>
-      </c>
-      <c r="U23" t="n">
-        <v>0</v>
-      </c>
-      <c r="V23" t="n">
-        <v>0</v>
-      </c>
-      <c r="W23" t="n">
-        <v>0</v>
-      </c>
-      <c r="X23" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y23" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD23" t="inlineStr"/>
-      <c r="AE23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG23" t="n">
-        <v>2</v>
-      </c>
-      <c r="AH23" t="n">
-        <v>85</v>
-      </c>
-      <c r="AI23" t="inlineStr"/>
-      <c r="AJ23" t="n">
-        <v>-85</v>
-      </c>
-      <c r="AK23" t="inlineStr"/>
-      <c r="AL23" t="inlineStr"/>
-      <c r="AM23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN23" t="inlineStr"/>
-      <c r="AO23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP23" t="inlineStr"/>
-      <c r="AQ23" t="inlineStr"/>
-      <c r="AR23" t="inlineStr"/>
-      <c r="AS23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT23" t="inlineStr"/>
-      <c r="AU23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
-        <v>24</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>32097</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
-      <c r="I24" t="inlineStr"/>
-      <c r="J24" t="n">
-        <v>0</v>
-      </c>
-      <c r="K24" t="n">
-        <v>0</v>
-      </c>
-      <c r="L24" t="n">
-        <v>0</v>
-      </c>
-      <c r="M24" t="n">
-        <v>0</v>
-      </c>
-      <c r="N24" t="n">
-        <v>0</v>
-      </c>
-      <c r="O24" t="n">
-        <v>0</v>
-      </c>
-      <c r="P24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q24" t="n">
-        <v>0</v>
-      </c>
-      <c r="R24" t="n">
-        <v>0</v>
-      </c>
-      <c r="S24" t="n">
-        <v>0</v>
-      </c>
-      <c r="T24" t="n">
-        <v>0</v>
-      </c>
-      <c r="U24" t="n">
-        <v>0</v>
-      </c>
-      <c r="V24" t="n">
-        <v>0</v>
-      </c>
-      <c r="W24" t="n">
-        <v>0</v>
-      </c>
-      <c r="X24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD24" t="inlineStr"/>
-      <c r="AE24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG24" t="n">
-        <v>2</v>
-      </c>
-      <c r="AH24" t="n">
-        <v>80</v>
-      </c>
-      <c r="AI24" t="inlineStr"/>
-      <c r="AJ24" t="n">
-        <v>-80</v>
-      </c>
-      <c r="AK24" t="inlineStr"/>
-      <c r="AL24" t="inlineStr"/>
-      <c r="AM24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN24" t="inlineStr"/>
-      <c r="AO24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP24" t="inlineStr"/>
-      <c r="AQ24" t="inlineStr"/>
-      <c r="AR24" t="inlineStr"/>
-      <c r="AS24" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT24" t="inlineStr"/>
-      <c r="AU24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
-        <v>25</v>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>32545</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
-      <c r="I25" t="inlineStr"/>
-      <c r="J25" t="n">
-        <v>0</v>
-      </c>
-      <c r="K25" t="n">
-        <v>0</v>
-      </c>
-      <c r="L25" t="n">
-        <v>0</v>
-      </c>
-      <c r="M25" t="n">
-        <v>0</v>
-      </c>
-      <c r="N25" t="n">
-        <v>0</v>
-      </c>
-      <c r="O25" t="n">
-        <v>0</v>
-      </c>
-      <c r="P25" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q25" t="n">
-        <v>0</v>
-      </c>
-      <c r="R25" t="n">
-        <v>0</v>
-      </c>
-      <c r="S25" t="n">
-        <v>0</v>
-      </c>
-      <c r="T25" t="n">
-        <v>0</v>
-      </c>
-      <c r="U25" t="n">
-        <v>0</v>
-      </c>
-      <c r="V25" t="n">
-        <v>0</v>
-      </c>
-      <c r="W25" t="n">
-        <v>0</v>
-      </c>
-      <c r="X25" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y25" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD25" t="inlineStr"/>
-      <c r="AE25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG25" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH25" t="n">
-        <v>40</v>
-      </c>
-      <c r="AI25" t="inlineStr"/>
-      <c r="AJ25" t="n">
-        <v>-40</v>
-      </c>
-      <c r="AK25" t="inlineStr"/>
-      <c r="AL25" t="inlineStr"/>
-      <c r="AM25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN25" t="inlineStr"/>
-      <c r="AO25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP25" t="inlineStr"/>
-      <c r="AQ25" t="inlineStr"/>
-      <c r="AR25" t="inlineStr"/>
-      <c r="AS25" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT25" t="inlineStr"/>
-      <c r="AU25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
-        <v>26</v>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>32563</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
-      <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr"/>
-      <c r="J26" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" t="n">
-        <v>0</v>
-      </c>
-      <c r="L26" t="n">
-        <v>0</v>
-      </c>
-      <c r="M26" t="n">
-        <v>0</v>
-      </c>
-      <c r="N26" t="n">
-        <v>0</v>
-      </c>
-      <c r="O26" t="n">
-        <v>0</v>
-      </c>
-      <c r="P26" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q26" t="n">
-        <v>0</v>
-      </c>
-      <c r="R26" t="n">
-        <v>0</v>
-      </c>
-      <c r="S26" t="n">
-        <v>0</v>
-      </c>
-      <c r="T26" t="n">
-        <v>0</v>
-      </c>
-      <c r="U26" t="n">
-        <v>0</v>
-      </c>
-      <c r="V26" t="n">
-        <v>0</v>
-      </c>
-      <c r="W26" t="n">
-        <v>0</v>
-      </c>
-      <c r="X26" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y26" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD26" t="inlineStr"/>
-      <c r="AE26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG26" t="n">
-        <v>5</v>
-      </c>
-      <c r="AH26" t="n">
-        <v>193</v>
-      </c>
-      <c r="AI26" t="inlineStr"/>
-      <c r="AJ26" t="n">
-        <v>-193</v>
-      </c>
-      <c r="AK26" t="inlineStr"/>
-      <c r="AL26" t="inlineStr"/>
-      <c r="AM26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN26" t="inlineStr"/>
-      <c r="AO26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP26" t="inlineStr"/>
-      <c r="AQ26" t="inlineStr"/>
-      <c r="AR26" t="inlineStr"/>
-      <c r="AS26" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT26" t="inlineStr"/>
-      <c r="AU26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
-        <v>27</v>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>32667</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr"/>
-      <c r="J27" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" t="n">
-        <v>0</v>
-      </c>
-      <c r="L27" t="n">
-        <v>0</v>
-      </c>
-      <c r="M27" t="n">
-        <v>0</v>
-      </c>
-      <c r="N27" t="n">
-        <v>0</v>
-      </c>
-      <c r="O27" t="n">
-        <v>0</v>
-      </c>
-      <c r="P27" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q27" t="n">
-        <v>0</v>
-      </c>
-      <c r="R27" t="n">
-        <v>0</v>
-      </c>
-      <c r="S27" t="n">
-        <v>0</v>
-      </c>
-      <c r="T27" t="n">
-        <v>0</v>
-      </c>
-      <c r="U27" t="n">
-        <v>0</v>
-      </c>
-      <c r="V27" t="n">
-        <v>0</v>
-      </c>
-      <c r="W27" t="n">
-        <v>0</v>
-      </c>
-      <c r="X27" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y27" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD27" t="inlineStr"/>
-      <c r="AE27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG27" t="n">
-        <v>5</v>
-      </c>
-      <c r="AH27" t="n">
-        <v>215</v>
-      </c>
-      <c r="AI27" t="inlineStr"/>
-      <c r="AJ27" t="n">
-        <v>-215</v>
-      </c>
-      <c r="AK27" t="inlineStr"/>
-      <c r="AL27" t="inlineStr"/>
-      <c r="AM27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN27" t="inlineStr"/>
-      <c r="AO27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP27" t="inlineStr"/>
-      <c r="AQ27" t="inlineStr"/>
-      <c r="AR27" t="inlineStr"/>
-      <c r="AS27" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT27" t="inlineStr"/>
-      <c r="AU27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
-        <v>28</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>32672</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
-      <c r="H28" t="inlineStr"/>
-      <c r="I28" t="inlineStr"/>
-      <c r="J28" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" t="n">
-        <v>0</v>
-      </c>
-      <c r="M28" t="n">
-        <v>0</v>
-      </c>
-      <c r="N28" t="n">
-        <v>0</v>
-      </c>
-      <c r="O28" t="n">
-        <v>0</v>
-      </c>
-      <c r="P28" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q28" t="n">
-        <v>0</v>
-      </c>
-      <c r="R28" t="n">
-        <v>0</v>
-      </c>
-      <c r="S28" t="n">
-        <v>0</v>
-      </c>
-      <c r="T28" t="n">
-        <v>0</v>
-      </c>
-      <c r="U28" t="n">
-        <v>0</v>
-      </c>
-      <c r="V28" t="n">
-        <v>0</v>
-      </c>
-      <c r="W28" t="n">
-        <v>0</v>
-      </c>
-      <c r="X28" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y28" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD28" t="inlineStr"/>
-      <c r="AE28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG28" t="n">
-        <v>3</v>
-      </c>
-      <c r="AH28" t="n">
-        <v>130</v>
-      </c>
-      <c r="AI28" t="inlineStr"/>
-      <c r="AJ28" t="n">
-        <v>-130</v>
-      </c>
-      <c r="AK28" t="inlineStr"/>
-      <c r="AL28" t="inlineStr"/>
-      <c r="AM28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN28" t="inlineStr"/>
-      <c r="AO28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP28" t="inlineStr"/>
-      <c r="AQ28" t="inlineStr"/>
-      <c r="AR28" t="inlineStr"/>
-      <c r="AS28" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT28" t="inlineStr"/>
-      <c r="AU28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
-        <v>29</v>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>32903</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr"/>
-      <c r="I29" t="inlineStr"/>
-      <c r="J29" t="n">
-        <v>0</v>
-      </c>
-      <c r="K29" t="n">
-        <v>0</v>
-      </c>
-      <c r="L29" t="n">
-        <v>0</v>
-      </c>
-      <c r="M29" t="n">
-        <v>0</v>
-      </c>
-      <c r="N29" t="n">
-        <v>0</v>
-      </c>
-      <c r="O29" t="n">
-        <v>0</v>
-      </c>
-      <c r="P29" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q29" t="n">
-        <v>0</v>
-      </c>
-      <c r="R29" t="n">
-        <v>0</v>
-      </c>
-      <c r="S29" t="n">
-        <v>0</v>
-      </c>
-      <c r="T29" t="n">
-        <v>0</v>
-      </c>
-      <c r="U29" t="n">
-        <v>0</v>
-      </c>
-      <c r="V29" t="n">
-        <v>0</v>
-      </c>
-      <c r="W29" t="n">
-        <v>0</v>
-      </c>
-      <c r="X29" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y29" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD29" t="inlineStr"/>
-      <c r="AE29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG29" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH29" t="n">
-        <v>50</v>
-      </c>
-      <c r="AI29" t="inlineStr"/>
-      <c r="AJ29" t="n">
-        <v>-50</v>
-      </c>
-      <c r="AK29" t="inlineStr"/>
-      <c r="AL29" t="inlineStr"/>
-      <c r="AM29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN29" t="inlineStr"/>
-      <c r="AO29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP29" t="inlineStr"/>
-      <c r="AQ29" t="inlineStr"/>
-      <c r="AR29" t="inlineStr"/>
-      <c r="AS29" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT29" t="inlineStr"/>
-      <c r="AU29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
-        <v>30</v>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>33003</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr"/>
-      <c r="G30" t="inlineStr"/>
-      <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
-      <c r="J30" t="n">
-        <v>0</v>
-      </c>
-      <c r="K30" t="n">
-        <v>0</v>
-      </c>
-      <c r="L30" t="n">
-        <v>0</v>
-      </c>
-      <c r="M30" t="n">
-        <v>0</v>
-      </c>
-      <c r="N30" t="n">
-        <v>0</v>
-      </c>
-      <c r="O30" t="n">
-        <v>0</v>
-      </c>
-      <c r="P30" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q30" t="n">
-        <v>0</v>
-      </c>
-      <c r="R30" t="n">
-        <v>0</v>
-      </c>
-      <c r="S30" t="n">
-        <v>0</v>
-      </c>
-      <c r="T30" t="n">
-        <v>0</v>
-      </c>
-      <c r="U30" t="n">
-        <v>0</v>
-      </c>
-      <c r="V30" t="n">
-        <v>0</v>
-      </c>
-      <c r="W30" t="n">
-        <v>0</v>
-      </c>
-      <c r="X30" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y30" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD30" t="inlineStr"/>
-      <c r="AE30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG30" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH30" t="n">
-        <v>45</v>
-      </c>
-      <c r="AI30" t="inlineStr"/>
-      <c r="AJ30" t="n">
-        <v>-45</v>
-      </c>
-      <c r="AK30" t="inlineStr"/>
-      <c r="AL30" t="inlineStr"/>
-      <c r="AM30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN30" t="inlineStr"/>
-      <c r="AO30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP30" t="inlineStr"/>
-      <c r="AQ30" t="inlineStr"/>
-      <c r="AR30" t="inlineStr"/>
-      <c r="AS30" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT30" t="inlineStr"/>
-      <c r="AU30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="n">
-        <v>31</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>33150</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr"/>
-      <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr"/>
-      <c r="J31" t="n">
-        <v>0</v>
-      </c>
-      <c r="K31" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" t="n">
-        <v>0</v>
-      </c>
-      <c r="M31" t="n">
-        <v>0</v>
-      </c>
-      <c r="N31" t="n">
-        <v>0</v>
-      </c>
-      <c r="O31" t="n">
-        <v>0</v>
-      </c>
-      <c r="P31" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q31" t="n">
-        <v>0</v>
-      </c>
-      <c r="R31" t="n">
-        <v>0</v>
-      </c>
-      <c r="S31" t="n">
-        <v>0</v>
-      </c>
-      <c r="T31" t="n">
-        <v>0</v>
-      </c>
-      <c r="U31" t="n">
-        <v>0</v>
-      </c>
-      <c r="V31" t="n">
-        <v>0</v>
-      </c>
-      <c r="W31" t="n">
-        <v>0</v>
-      </c>
-      <c r="X31" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y31" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD31" t="inlineStr"/>
-      <c r="AE31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG31" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH31" t="n">
-        <v>33</v>
-      </c>
-      <c r="AI31" t="inlineStr"/>
-      <c r="AJ31" t="n">
-        <v>-33</v>
-      </c>
-      <c r="AK31" t="inlineStr"/>
-      <c r="AL31" t="inlineStr"/>
-      <c r="AM31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN31" t="inlineStr"/>
-      <c r="AO31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP31" t="inlineStr"/>
-      <c r="AQ31" t="inlineStr"/>
-      <c r="AR31" t="inlineStr"/>
-      <c r="AS31" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT31" t="inlineStr"/>
-      <c r="AU31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>32</v>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>33272</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr"/>
-      <c r="G32" t="inlineStr"/>
-      <c r="H32" t="inlineStr"/>
-      <c r="I32" t="inlineStr"/>
-      <c r="J32" t="n">
-        <v>0</v>
-      </c>
-      <c r="K32" t="n">
-        <v>0</v>
-      </c>
-      <c r="L32" t="n">
-        <v>0</v>
-      </c>
-      <c r="M32" t="n">
-        <v>0</v>
-      </c>
-      <c r="N32" t="n">
-        <v>0</v>
-      </c>
-      <c r="O32" t="n">
-        <v>0</v>
-      </c>
-      <c r="P32" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q32" t="n">
-        <v>0</v>
-      </c>
-      <c r="R32" t="n">
-        <v>0</v>
-      </c>
-      <c r="S32" t="n">
-        <v>0</v>
-      </c>
-      <c r="T32" t="n">
-        <v>0</v>
-      </c>
-      <c r="U32" t="n">
-        <v>0</v>
-      </c>
-      <c r="V32" t="n">
-        <v>0</v>
-      </c>
-      <c r="W32" t="n">
-        <v>0</v>
-      </c>
-      <c r="X32" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y32" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD32" t="inlineStr"/>
-      <c r="AE32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG32" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH32" t="n">
-        <v>33</v>
-      </c>
-      <c r="AI32" t="inlineStr"/>
-      <c r="AJ32" t="n">
-        <v>-33</v>
-      </c>
-      <c r="AK32" t="inlineStr"/>
-      <c r="AL32" t="inlineStr"/>
-      <c r="AM32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN32" t="inlineStr"/>
-      <c r="AO32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP32" t="inlineStr"/>
-      <c r="AQ32" t="inlineStr"/>
-      <c r="AR32" t="inlineStr"/>
-      <c r="AS32" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT32" t="inlineStr"/>
-      <c r="AU32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="n">
-        <v>33</v>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>33278</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr"/>
-      <c r="G33" t="inlineStr"/>
-      <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
-      <c r="J33" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" t="n">
-        <v>0</v>
-      </c>
-      <c r="L33" t="n">
-        <v>0</v>
-      </c>
-      <c r="M33" t="n">
-        <v>0</v>
-      </c>
-      <c r="N33" t="n">
-        <v>0</v>
-      </c>
-      <c r="O33" t="n">
-        <v>0</v>
-      </c>
-      <c r="P33" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q33" t="n">
-        <v>0</v>
-      </c>
-      <c r="R33" t="n">
-        <v>0</v>
-      </c>
-      <c r="S33" t="n">
-        <v>0</v>
-      </c>
-      <c r="T33" t="n">
-        <v>0</v>
-      </c>
-      <c r="U33" t="n">
-        <v>0</v>
-      </c>
-      <c r="V33" t="n">
-        <v>0</v>
-      </c>
-      <c r="W33" t="n">
-        <v>0</v>
-      </c>
-      <c r="X33" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y33" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD33" t="inlineStr"/>
-      <c r="AE33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG33" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH33" t="n">
-        <v>33</v>
-      </c>
-      <c r="AI33" t="inlineStr"/>
-      <c r="AJ33" t="n">
-        <v>-33</v>
-      </c>
-      <c r="AK33" t="inlineStr"/>
-      <c r="AL33" t="inlineStr"/>
-      <c r="AM33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN33" t="inlineStr"/>
-      <c r="AO33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP33" t="inlineStr"/>
-      <c r="AQ33" t="inlineStr"/>
-      <c r="AR33" t="inlineStr"/>
-      <c r="AS33" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT33" t="inlineStr"/>
-      <c r="AU33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="n">
-        <v>34</v>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>33675</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
-      <c r="J34" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" t="n">
-        <v>0</v>
-      </c>
-      <c r="L34" t="n">
-        <v>0</v>
-      </c>
-      <c r="M34" t="n">
-        <v>0</v>
-      </c>
-      <c r="N34" t="n">
-        <v>0</v>
-      </c>
-      <c r="O34" t="n">
-        <v>0</v>
-      </c>
-      <c r="P34" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q34" t="n">
-        <v>0</v>
-      </c>
-      <c r="R34" t="n">
-        <v>0</v>
-      </c>
-      <c r="S34" t="n">
-        <v>0</v>
-      </c>
-      <c r="T34" t="n">
-        <v>0</v>
-      </c>
-      <c r="U34" t="n">
-        <v>0</v>
-      </c>
-      <c r="V34" t="n">
-        <v>0</v>
-      </c>
-      <c r="W34" t="n">
-        <v>0</v>
-      </c>
-      <c r="X34" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y34" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD34" t="inlineStr"/>
-      <c r="AE34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG34" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH34" t="n">
-        <v>40</v>
-      </c>
-      <c r="AI34" t="inlineStr"/>
-      <c r="AJ34" t="n">
-        <v>-40</v>
-      </c>
-      <c r="AK34" t="inlineStr"/>
-      <c r="AL34" t="inlineStr"/>
-      <c r="AM34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN34" t="inlineStr"/>
-      <c r="AO34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP34" t="inlineStr"/>
-      <c r="AQ34" t="inlineStr"/>
-      <c r="AR34" t="inlineStr"/>
-      <c r="AS34" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT34" t="inlineStr"/>
-      <c r="AU34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="n">
-        <v>35</v>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>33682</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="n">
-        <v>0</v>
-      </c>
-      <c r="K35" t="n">
-        <v>0</v>
-      </c>
-      <c r="L35" t="n">
-        <v>0</v>
-      </c>
-      <c r="M35" t="n">
-        <v>0</v>
-      </c>
-      <c r="N35" t="n">
-        <v>0</v>
-      </c>
-      <c r="O35" t="n">
-        <v>0</v>
-      </c>
-      <c r="P35" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q35" t="n">
-        <v>0</v>
-      </c>
-      <c r="R35" t="n">
-        <v>0</v>
-      </c>
-      <c r="S35" t="n">
-        <v>0</v>
-      </c>
-      <c r="T35" t="n">
-        <v>0</v>
-      </c>
-      <c r="U35" t="n">
-        <v>0</v>
-      </c>
-      <c r="V35" t="n">
-        <v>0</v>
-      </c>
-      <c r="W35" t="n">
-        <v>0</v>
-      </c>
-      <c r="X35" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y35" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD35" t="inlineStr"/>
-      <c r="AE35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG35" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH35" t="n">
-        <v>33</v>
-      </c>
-      <c r="AI35" t="inlineStr"/>
-      <c r="AJ35" t="n">
-        <v>-33</v>
-      </c>
-      <c r="AK35" t="inlineStr"/>
-      <c r="AL35" t="inlineStr"/>
-      <c r="AM35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN35" t="inlineStr"/>
-      <c r="AO35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP35" t="inlineStr"/>
-      <c r="AQ35" t="inlineStr"/>
-      <c r="AR35" t="inlineStr"/>
-      <c r="AS35" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT35" t="inlineStr"/>
-      <c r="AU35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>36</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>33683</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
-      <c r="G36" t="inlineStr"/>
-      <c r="H36" t="inlineStr"/>
-      <c r="I36" t="inlineStr"/>
-      <c r="J36" t="n">
-        <v>0</v>
-      </c>
-      <c r="K36" t="n">
-        <v>0</v>
-      </c>
-      <c r="L36" t="n">
-        <v>0</v>
-      </c>
-      <c r="M36" t="n">
-        <v>0</v>
-      </c>
-      <c r="N36" t="n">
-        <v>0</v>
-      </c>
-      <c r="O36" t="n">
-        <v>0</v>
-      </c>
-      <c r="P36" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q36" t="n">
-        <v>0</v>
-      </c>
-      <c r="R36" t="n">
-        <v>0</v>
-      </c>
-      <c r="S36" t="n">
-        <v>0</v>
-      </c>
-      <c r="T36" t="n">
-        <v>0</v>
-      </c>
-      <c r="U36" t="n">
-        <v>0</v>
-      </c>
-      <c r="V36" t="n">
-        <v>0</v>
-      </c>
-      <c r="W36" t="n">
-        <v>0</v>
-      </c>
-      <c r="X36" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y36" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD36" t="inlineStr"/>
-      <c r="AE36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG36" t="n">
-        <v>2</v>
-      </c>
-      <c r="AH36" t="n">
-        <v>80</v>
-      </c>
-      <c r="AI36" t="inlineStr"/>
-      <c r="AJ36" t="n">
-        <v>-80</v>
-      </c>
-      <c r="AK36" t="inlineStr"/>
-      <c r="AL36" t="inlineStr"/>
-      <c r="AM36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN36" t="inlineStr"/>
-      <c r="AO36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP36" t="inlineStr"/>
-      <c r="AQ36" t="inlineStr"/>
-      <c r="AR36" t="inlineStr"/>
-      <c r="AS36" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT36" t="inlineStr"/>
-      <c r="AU36" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="n">
-        <v>37</v>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>33687</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr"/>
-      <c r="G37" t="inlineStr"/>
-      <c r="H37" t="inlineStr"/>
-      <c r="I37" t="inlineStr"/>
-      <c r="J37" t="n">
-        <v>0</v>
-      </c>
-      <c r="K37" t="n">
-        <v>0</v>
-      </c>
-      <c r="L37" t="n">
-        <v>0</v>
-      </c>
-      <c r="M37" t="n">
-        <v>0</v>
-      </c>
-      <c r="N37" t="n">
-        <v>0</v>
-      </c>
-      <c r="O37" t="n">
-        <v>0</v>
-      </c>
-      <c r="P37" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q37" t="n">
-        <v>0</v>
-      </c>
-      <c r="R37" t="n">
-        <v>0</v>
-      </c>
-      <c r="S37" t="n">
-        <v>0</v>
-      </c>
-      <c r="T37" t="n">
-        <v>0</v>
-      </c>
-      <c r="U37" t="n">
-        <v>0</v>
-      </c>
-      <c r="V37" t="n">
-        <v>0</v>
-      </c>
-      <c r="W37" t="n">
-        <v>0</v>
-      </c>
-      <c r="X37" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y37" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD37" t="inlineStr"/>
-      <c r="AE37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG37" t="n">
-        <v>3</v>
-      </c>
-      <c r="AH37" t="n">
-        <v>113</v>
-      </c>
-      <c r="AI37" t="inlineStr"/>
-      <c r="AJ37" t="n">
-        <v>-113</v>
-      </c>
-      <c r="AK37" t="inlineStr"/>
-      <c r="AL37" t="inlineStr"/>
-      <c r="AM37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN37" t="inlineStr"/>
-      <c r="AO37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP37" t="inlineStr"/>
-      <c r="AQ37" t="inlineStr"/>
-      <c r="AR37" t="inlineStr"/>
-      <c r="AS37" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT37" t="inlineStr"/>
-      <c r="AU37" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="n">
-        <v>38</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>33689</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr"/>
-      <c r="J38" t="n">
-        <v>0</v>
-      </c>
-      <c r="K38" t="n">
-        <v>0</v>
-      </c>
-      <c r="L38" t="n">
-        <v>0</v>
-      </c>
-      <c r="M38" t="n">
-        <v>0</v>
-      </c>
-      <c r="N38" t="n">
-        <v>0</v>
-      </c>
-      <c r="O38" t="n">
-        <v>0</v>
-      </c>
-      <c r="P38" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q38" t="n">
-        <v>0</v>
-      </c>
-      <c r="R38" t="n">
-        <v>0</v>
-      </c>
-      <c r="S38" t="n">
-        <v>0</v>
-      </c>
-      <c r="T38" t="n">
-        <v>0</v>
-      </c>
-      <c r="U38" t="n">
-        <v>0</v>
-      </c>
-      <c r="V38" t="n">
-        <v>0</v>
-      </c>
-      <c r="W38" t="n">
-        <v>0</v>
-      </c>
-      <c r="X38" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y38" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD38" t="inlineStr"/>
-      <c r="AE38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG38" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH38" t="n">
-        <v>33</v>
-      </c>
-      <c r="AI38" t="inlineStr"/>
-      <c r="AJ38" t="n">
-        <v>-33</v>
-      </c>
-      <c r="AK38" t="inlineStr"/>
-      <c r="AL38" t="inlineStr"/>
-      <c r="AM38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN38" t="inlineStr"/>
-      <c r="AO38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP38" t="inlineStr"/>
-      <c r="AQ38" t="inlineStr"/>
-      <c r="AR38" t="inlineStr"/>
-      <c r="AS38" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT38" t="inlineStr"/>
-      <c r="AU38" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="n">
-        <v>39</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>33770</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
-      <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
-      <c r="H39" t="inlineStr"/>
-      <c r="I39" t="inlineStr"/>
-      <c r="J39" t="n">
-        <v>0</v>
-      </c>
-      <c r="K39" t="n">
-        <v>0</v>
-      </c>
-      <c r="L39" t="n">
-        <v>0</v>
-      </c>
-      <c r="M39" t="n">
-        <v>0</v>
-      </c>
-      <c r="N39" t="n">
-        <v>0</v>
-      </c>
-      <c r="O39" t="n">
-        <v>0</v>
-      </c>
-      <c r="P39" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q39" t="n">
-        <v>0</v>
-      </c>
-      <c r="R39" t="n">
-        <v>0</v>
-      </c>
-      <c r="S39" t="n">
-        <v>0</v>
-      </c>
-      <c r="T39" t="n">
-        <v>0</v>
-      </c>
-      <c r="U39" t="n">
-        <v>0</v>
-      </c>
-      <c r="V39" t="n">
-        <v>0</v>
-      </c>
-      <c r="W39" t="n">
-        <v>0</v>
-      </c>
-      <c r="X39" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y39" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD39" t="inlineStr"/>
-      <c r="AE39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG39" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH39" t="n">
-        <v>45</v>
-      </c>
-      <c r="AI39" t="inlineStr"/>
-      <c r="AJ39" t="n">
-        <v>-45</v>
-      </c>
-      <c r="AK39" t="inlineStr"/>
-      <c r="AL39" t="inlineStr"/>
-      <c r="AM39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN39" t="inlineStr"/>
-      <c r="AO39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP39" t="inlineStr"/>
-      <c r="AQ39" t="inlineStr"/>
-      <c r="AR39" t="inlineStr"/>
-      <c r="AS39" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT39" t="inlineStr"/>
-      <c r="AU39" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="n">
-        <v>40</v>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>33867</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr"/>
-      <c r="G40" t="inlineStr"/>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr"/>
-      <c r="J40" t="n">
-        <v>0</v>
-      </c>
-      <c r="K40" t="n">
-        <v>0</v>
-      </c>
-      <c r="L40" t="n">
-        <v>0</v>
-      </c>
-      <c r="M40" t="n">
-        <v>0</v>
-      </c>
-      <c r="N40" t="n">
-        <v>0</v>
-      </c>
-      <c r="O40" t="n">
-        <v>0</v>
-      </c>
-      <c r="P40" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q40" t="n">
-        <v>0</v>
-      </c>
-      <c r="R40" t="n">
-        <v>0</v>
-      </c>
-      <c r="S40" t="n">
-        <v>0</v>
-      </c>
-      <c r="T40" t="n">
-        <v>0</v>
-      </c>
-      <c r="U40" t="n">
-        <v>0</v>
-      </c>
-      <c r="V40" t="n">
-        <v>0</v>
-      </c>
-      <c r="W40" t="n">
-        <v>0</v>
-      </c>
-      <c r="X40" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y40" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD40" t="inlineStr"/>
-      <c r="AE40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG40" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH40" t="n">
-        <v>40</v>
-      </c>
-      <c r="AI40" t="inlineStr"/>
-      <c r="AJ40" t="n">
-        <v>-40</v>
-      </c>
-      <c r="AK40" t="inlineStr"/>
-      <c r="AL40" t="inlineStr"/>
-      <c r="AM40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN40" t="inlineStr"/>
-      <c r="AO40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP40" t="inlineStr"/>
-      <c r="AQ40" t="inlineStr"/>
-      <c r="AR40" t="inlineStr"/>
-      <c r="AS40" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT40" t="inlineStr"/>
-      <c r="AU40" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>41</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>33871</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr"/>
-      <c r="G41" t="inlineStr"/>
-      <c r="H41" t="inlineStr"/>
-      <c r="I41" t="inlineStr"/>
-      <c r="J41" t="n">
-        <v>0</v>
-      </c>
-      <c r="K41" t="n">
-        <v>0</v>
-      </c>
-      <c r="L41" t="n">
-        <v>0</v>
-      </c>
-      <c r="M41" t="n">
-        <v>0</v>
-      </c>
-      <c r="N41" t="n">
-        <v>0</v>
-      </c>
-      <c r="O41" t="n">
-        <v>0</v>
-      </c>
-      <c r="P41" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q41" t="n">
-        <v>0</v>
-      </c>
-      <c r="R41" t="n">
-        <v>0</v>
-      </c>
-      <c r="S41" t="n">
-        <v>0</v>
-      </c>
-      <c r="T41" t="n">
-        <v>0</v>
-      </c>
-      <c r="U41" t="n">
-        <v>0</v>
-      </c>
-      <c r="V41" t="n">
-        <v>0</v>
-      </c>
-      <c r="W41" t="n">
-        <v>0</v>
-      </c>
-      <c r="X41" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y41" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD41" t="inlineStr"/>
-      <c r="AE41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG41" t="n">
-        <v>3</v>
-      </c>
-      <c r="AH41" t="n">
-        <v>123</v>
-      </c>
-      <c r="AI41" t="inlineStr"/>
-      <c r="AJ41" t="n">
-        <v>-123</v>
-      </c>
-      <c r="AK41" t="inlineStr"/>
-      <c r="AL41" t="inlineStr"/>
-      <c r="AM41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN41" t="inlineStr"/>
-      <c r="AO41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP41" t="inlineStr"/>
-      <c r="AQ41" t="inlineStr"/>
-      <c r="AR41" t="inlineStr"/>
-      <c r="AS41" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT41" t="inlineStr"/>
-      <c r="AU41" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>42</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>33891</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr"/>
-      <c r="G42" t="inlineStr"/>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr"/>
-      <c r="J42" t="n">
-        <v>0</v>
-      </c>
-      <c r="K42" t="n">
-        <v>0</v>
-      </c>
-      <c r="L42" t="n">
-        <v>0</v>
-      </c>
-      <c r="M42" t="n">
-        <v>0</v>
-      </c>
-      <c r="N42" t="n">
-        <v>0</v>
-      </c>
-      <c r="O42" t="n">
-        <v>0</v>
-      </c>
-      <c r="P42" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q42" t="n">
-        <v>0</v>
-      </c>
-      <c r="R42" t="n">
-        <v>0</v>
-      </c>
-      <c r="S42" t="n">
-        <v>0</v>
-      </c>
-      <c r="T42" t="n">
-        <v>0</v>
-      </c>
-      <c r="U42" t="n">
-        <v>0</v>
-      </c>
-      <c r="V42" t="n">
-        <v>0</v>
-      </c>
-      <c r="W42" t="n">
-        <v>0</v>
-      </c>
-      <c r="X42" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y42" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD42" t="inlineStr"/>
-      <c r="AE42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG42" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH42" t="n">
-        <v>33</v>
-      </c>
-      <c r="AI42" t="inlineStr"/>
-      <c r="AJ42" t="n">
-        <v>-33</v>
-      </c>
-      <c r="AK42" t="inlineStr"/>
-      <c r="AL42" t="inlineStr"/>
-      <c r="AM42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN42" t="inlineStr"/>
-      <c r="AO42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP42" t="inlineStr"/>
-      <c r="AQ42" t="inlineStr"/>
-      <c r="AR42" t="inlineStr"/>
-      <c r="AS42" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT42" t="inlineStr"/>
-      <c r="AU42" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>43</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>3095</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>33984</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
-      <c r="G43" t="inlineStr"/>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr"/>
-      <c r="J43" t="n">
-        <v>0</v>
-      </c>
-      <c r="K43" t="n">
-        <v>0</v>
-      </c>
-      <c r="L43" t="n">
-        <v>0</v>
-      </c>
-      <c r="M43" t="n">
-        <v>0</v>
-      </c>
-      <c r="N43" t="n">
-        <v>0</v>
-      </c>
-      <c r="O43" t="n">
-        <v>0</v>
-      </c>
-      <c r="P43" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q43" t="n">
-        <v>0</v>
-      </c>
-      <c r="R43" t="n">
-        <v>0</v>
-      </c>
-      <c r="S43" t="n">
-        <v>0</v>
-      </c>
-      <c r="T43" t="n">
-        <v>0</v>
-      </c>
-      <c r="U43" t="n">
-        <v>0</v>
-      </c>
-      <c r="V43" t="n">
-        <v>0</v>
-      </c>
-      <c r="W43" t="n">
-        <v>0</v>
-      </c>
-      <c r="X43" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y43" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD43" t="inlineStr"/>
-      <c r="AE43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG43" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH43" t="n">
-        <v>33</v>
-      </c>
-      <c r="AI43" t="inlineStr"/>
-      <c r="AJ43" t="n">
-        <v>-33</v>
-      </c>
-      <c r="AK43" t="inlineStr"/>
-      <c r="AL43" t="inlineStr"/>
-      <c r="AM43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN43" t="inlineStr"/>
-      <c r="AO43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AP43" t="inlineStr"/>
-      <c r="AQ43" t="inlineStr"/>
-      <c r="AR43" t="inlineStr"/>
-      <c r="AS43" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT43" t="inlineStr"/>
-      <c r="AU43" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr filterMode="0">

</xml_diff>